<commit_message>
Implemented Re-use gift card
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupTA635.xlsx
+++ b/src/test/resources/data/jdgroupTA635.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F0A522-C94E-4A15-83F0-A847D0250A97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458966A8-6064-4C3E-8C27-3A28ED2B59A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="70" activeTab="72" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33609,7 +33609,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38116,15 +38116,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -38273,6 +38264,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
@@ -38282,23 +38282,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -38315,4 +38298,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update TA635 to accomdate syncronization.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupTA635.xlsx
+++ b/src/test/resources/data/jdgroupTA635.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B209E06D-D6CB-4E1E-86F7-3BB703C3E361}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="69" activeTab="72"/>
   </bookViews>
   <sheets>
     <sheet name="EVS" sheetId="82" r:id="rId1"/>
@@ -114,12 +113,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -137,12 +136,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2300-000001000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2300-000002000000}">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -181,12 +180,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2400-000001000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -203,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2400-000002000000}">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -225,12 +224,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-5200-000001000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3291,7 +3290,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19">
     <font>
       <sz val="11"/>
@@ -4154,9 +4153,9 @@
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="4"/>
+    <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
   <dxfs count="319">
     <dxf>
@@ -7379,156 +7378,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="evs_SAP_OrderRelated++"/>
-      <sheetName val="evs_OrderStatusSearch++"/>
-      <sheetName val="URL++"/>
-      <sheetName val="EVS_Login_magento++"/>
-      <sheetName val="Login_magento++"/>
-      <sheetName val="Suites"/>
-      <sheetName val="IC"/>
-      <sheetName val="EVS"/>
-      <sheetName val="validatePaymentOption++"/>
-      <sheetName val="evs_RetriveOrderID++"/>
-      <sheetName val="evs_PayUPagePayment++"/>
-      <sheetName val="evs_CheckoutpaymentOption++"/>
-      <sheetName val="evs_GenerateOrderSAPnumber++"/>
-      <sheetName val="evs_DeliveryPopulation++"/>
-      <sheetName val="evs_AccountCreation++"/>
-      <sheetName val="evs_ProductSearch++"/>
-      <sheetName val="ProductSearch++"/>
-      <sheetName val="accountCreation++"/>
-      <sheetName val="parrallel_ic_Login++"/>
-      <sheetName val="evs_Login++"/>
-      <sheetName val="SapRSIGetDataFromSAPDB++"/>
-      <sheetName val="icInvalidEmailNewsLetter++"/>
-      <sheetName val="ic_SubscribeNewsletter++"/>
-      <sheetName val="evs_RemoveFromcart++"/>
-      <sheetName val="ic_RemoveFromcart++"/>
-      <sheetName val="IC_ClearWishList++"/>
-      <sheetName val="evs_ClearWishList++"/>
-      <sheetName val="evs_NavigetoWishlist++"/>
-      <sheetName val="ic_NavigetoWishlist++"/>
-      <sheetName val="Magento_UserInfoVerification++"/>
-      <sheetName val="IC_ProductsSortBy++"/>
-      <sheetName val="ic_SubscribeNews_DupliEmailID++"/>
-      <sheetName val="EnterSpouseInfor++"/>
-      <sheetName val="EnterContact++"/>
-      <sheetName val="CreditEnterAddressDetails++"/>
-      <sheetName val="CreditEnterEmploymentDetails++"/>
-      <sheetName val="EnterBasicDetails++"/>
-      <sheetName val="CreditStatusVerification++"/>
-      <sheetName val="CreditApp_NavigateFilter++"/>
-      <sheetName val="giftCardReport++"/>
-      <sheetName val="adminUserUpdate++"/>
-      <sheetName val="ICUpdateUser++"/>
-      <sheetName val="SapCustomer++"/>
-      <sheetName val="PayUPagePayment++"/>
-      <sheetName val="CheckoutpaymentOption++"/>
-      <sheetName val="deliveryPopulation++"/>
-      <sheetName val="RetrieveCustomerDetailsOld++"/>
-      <sheetName val="icGiftCardPurchase++"/>
-      <sheetName val="SAP_OrderRelated++"/>
-      <sheetName val="GenerateOrderSAPnumber++"/>
-      <sheetName val="OrderStatusSearch++"/>
-      <sheetName val="ic_RetriveOrderID++"/>
-      <sheetName val="evs_WishlistToCart++"/>
-      <sheetName val="IC_WishlistToCart++"/>
       <sheetName val="Products_Category"/>
-      <sheetName val="icRedeemGiftCard++"/>
-      <sheetName val="VeriyGiftcardUsableity++"/>
-      <sheetName val="ic_login++"/>
-      <sheetName val="ClearCart++"/>
-      <sheetName val="ic_invalidCredslogin++"/>
-      <sheetName val="SendWishlistToEmail++"/>
-      <sheetName val="icEmailWishlistverification++"/>
-      <sheetName val="DB_connection_master++"/>
-      <sheetName val="icGiftCardVerificationSender++"/>
-      <sheetName val="ic_CashDepositPayment++"/>
-      <sheetName val="CreateaccountBackend++"/>
-      <sheetName val="icSearchNoResultsReturned++"/>
-      <sheetName val="Russels"/>
-      <sheetName val="Login++"/>
-      <sheetName val="Bradlows"/>
-      <sheetName val="Rochester"/>
-      <sheetName val="Preferred Store"/>
-      <sheetName val="Sleepmasters"/>
-      <sheetName val="HiFiCorp"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7590,7 +7443,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7623,26 +7476,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7675,23 +7511,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7867,11 +7686,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView topLeftCell="H55" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -10275,146 +10094,146 @@
     <cfRule type="duplicateValues" dxfId="277" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H2" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I2" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="J2" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="K2" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="L2" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="N2" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="O2" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H3" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H4:H7" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="P2" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="M2" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G8" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="H9" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="H10" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="H11" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="H12" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="H13" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G14" location="'parallel_evs_Login++'!A1" display="parallel_evs_Login" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="H15" location="'evs_invalidCredslogin++'!A1" display="evs_invalidCredslogin" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="H16" location="'evs_invalidCredslogin++'!A1" display="evs_invalidCredslogin" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="H17" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="H18:H20" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="I17" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="I18:I20" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="L17" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K17" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="K18:K20" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="L18:L20" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="H21" location="'evs_Login++'!A1" display="evs_ForgotPassword" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="H22" location="'evs_Login++'!A1" display="evs_ForgotPasswordLink" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="H23" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="J24" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="H24" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="L24" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="G25" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="G26:G27" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="H25" location="'evs_CreateaccountBackend++'!A1" display="evs_CreateaccountBackend" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="H26:H27" location="'evs_CreateaccountBackend++'!A1" display="evs_CreateaccountBackend" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="I25" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="I26:I27" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="J25" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="J26:J27" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="H28" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="H29:H32" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="I28" location="'evs_UpdateUser++'!A1" display="evs_UpdateUser" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="I29:I32" location="'evs_UpdateUser++'!A1" display="evs_UpdateUser" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="J28" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="J29:J32" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="L28" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="L29:L32" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="M28" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="M29:M32" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="G33" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="H33" location="'evs_adminUserUpdate++'!A1" display="evs_adminUserUpdate" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="I33" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="J33" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="G34:G37" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="H34:H37" location="'evs_adminUserUpdate++'!A1" display="evs_adminUserUpdate" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="I34:I37" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="J34:J37" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="H39" location="'evs_NavigetoWishlist++'!A1" display="evs_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="H41:H42" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="K42" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="M42" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="L43" location="'evs_WishlistToCart++'!A1" display="evs_WishlistToCart" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="H44" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="H43" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="I41" location="'evs_ClearWishList++'!A1" display="evs_ClearWishList" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="J39" location="'evs_RemoveFromcart++'!A1" display="evs_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="I41:I44" location="'evs_RemoveFromcart++'!A1" display="evs_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="J43:J44" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="H40" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="K39" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="G45" location="'parrallel_ic_Login++'!A1" display="parrallel_ic_Login" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="J52" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="K52" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="L52" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="M52" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="O52" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="P52" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="N52" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="J53" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="K53" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="L53" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="M53" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="O53" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="P53" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="N53" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="H48:H51" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="H54" location="'evs_SubscribeNews_DupEmailID++'!A1" display="evs_SubscribeNews_DupEmailID" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="H55" location="'evs_InvalidEmailNewsLetter++'!A1" display="evs_InvalidEmailNewsLetter" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="H56" location="'evs_SubscribeNewsletter++'!A1" display="ic_SubscribeNewsletter" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="G48" location="'EVS_SapRSIGetDataFromSAPDB++'!A1" display="EVS_SapRSIGetDataFromSAPDB" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="G49:G51" location="'EVS_SapRSIGetDataFromSAPDB++'!A1" display="EVS_SapRSIGetDataFromSAPDB" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="I52" location="'evs_ProductSearch++'!A1" display="EVS_skuProduct" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="I53" location="'evs_ProductSearch++'!A1" display="EVS_skuProduct" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="G53" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="G54:G56" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="G52" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="H58" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="I58" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="J58" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="K58" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="M58" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="O58" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="P58" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="H57" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="H59" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="J57" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="K57" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="L57" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="N57" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="P57" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="Q57" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="R57" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="O57" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="J59" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="K59" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="L59" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="M59" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="O59" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="Q59" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="R59" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="N59" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="L58" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="M57" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="G57" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="G58" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="G59" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="H60" location="'evs_SubscribeNews_DupEmailID++'!A1" display="evs_SubscribeNews_DupEmailID" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="H61" location="'evs_InvalidEmailNewsLetter++'!A1" display="evs_InvalidEmailNewsLetter" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="H62" location="'evs_SubscribeNewsletter++'!A1" display="ic_SubscribeNewsletter" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="G60:G62" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="H63" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="J63" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="G63" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="H64" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{9AED98AB-9722-4589-ABF2-FB470B26F770}"/>
-    <hyperlink ref="G64" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal" xr:uid="{9371C671-4CDA-4A45-9458-A54C0E4E3A85}"/>
-    <hyperlink ref="J64" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{6C12052A-63B7-4F2C-8171-CF2864119E18}"/>
-    <hyperlink ref="K64" location="'evs_RedeemGiftCard++'!A1" display="evs_RedeemGiftCard" xr:uid="{E1A6302C-0689-4B04-AC21-115C2D085B2F}"/>
+    <hyperlink ref="H2" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="I2" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="J2" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="K2" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment"/>
+    <hyperlink ref="L2" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="N2" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="O2" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="H3" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation"/>
+    <hyperlink ref="H4:H7" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation"/>
+    <hyperlink ref="P2" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated"/>
+    <hyperlink ref="M2" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="G8" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H9" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H10" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H11" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H12" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H13" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="G14" location="'parallel_evs_Login++'!A1" display="parallel_evs_Login"/>
+    <hyperlink ref="H15" location="'evs_invalidCredslogin++'!A1" display="evs_invalidCredslogin"/>
+    <hyperlink ref="H16" location="'evs_invalidCredslogin++'!A1" display="evs_invalidCredslogin"/>
+    <hyperlink ref="H17" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation"/>
+    <hyperlink ref="H18:H20" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation"/>
+    <hyperlink ref="I17" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="I18:I20" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="L17" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="K17" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="K18:K20" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="L18:L20" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="H21" location="'evs_Login++'!A1" display="evs_ForgotPassword"/>
+    <hyperlink ref="H22" location="'evs_Login++'!A1" display="evs_ForgotPasswordLink"/>
+    <hyperlink ref="H23" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="J24" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H24" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="L24" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="G25" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="G26:G27" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H25" location="'evs_CreateaccountBackend++'!A1" display="evs_CreateaccountBackend"/>
+    <hyperlink ref="H26:H27" location="'evs_CreateaccountBackend++'!A1" display="evs_CreateaccountBackend"/>
+    <hyperlink ref="I25" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="I26:I27" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="J25" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="J26:J27" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="H28" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="H29:H32" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="I28" location="'evs_UpdateUser++'!A1" display="evs_UpdateUser"/>
+    <hyperlink ref="I29:I32" location="'evs_UpdateUser++'!A1" display="evs_UpdateUser"/>
+    <hyperlink ref="J28" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="J29:J32" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="L28" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="L29:L32" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="M28" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="M29:M32" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="G33" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H33" location="'evs_adminUserUpdate++'!A1" display="evs_adminUserUpdate"/>
+    <hyperlink ref="I33" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="J33" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="G34:G37" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H34:H37" location="'evs_adminUserUpdate++'!A1" display="evs_adminUserUpdate"/>
+    <hyperlink ref="I34:I37" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="J34:J37" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="H39" location="'evs_NavigetoWishlist++'!A1" display="evs_NavigetoWishlist"/>
+    <hyperlink ref="H41:H42" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="K42" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="M42" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="L43" location="'evs_WishlistToCart++'!A1" display="evs_WishlistToCart"/>
+    <hyperlink ref="H44" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H43" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="I41" location="'evs_ClearWishList++'!A1" display="evs_ClearWishList"/>
+    <hyperlink ref="J39" location="'evs_RemoveFromcart++'!A1" display="evs_RemoveFromcart"/>
+    <hyperlink ref="I41:I44" location="'evs_RemoveFromcart++'!A1" display="evs_RemoveFromcart"/>
+    <hyperlink ref="J43:J44" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H40" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="K39" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="G45" location="'parrallel_ic_Login++'!A1" display="parrallel_ic_Login"/>
+    <hyperlink ref="J52" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="K52" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="L52" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment"/>
+    <hyperlink ref="M52" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="O52" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="P52" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="N52" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="J53" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="K53" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="L53" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment"/>
+    <hyperlink ref="M53" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="O53" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="P53" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="N53" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H48:H51" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H54" location="'evs_SubscribeNews_DupEmailID++'!A1" display="evs_SubscribeNews_DupEmailID"/>
+    <hyperlink ref="H55" location="'evs_InvalidEmailNewsLetter++'!A1" display="evs_InvalidEmailNewsLetter"/>
+    <hyperlink ref="H56" location="'evs_SubscribeNewsletter++'!A1" display="ic_SubscribeNewsletter"/>
+    <hyperlink ref="G48" location="'EVS_SapRSIGetDataFromSAPDB++'!A1" display="EVS_SapRSIGetDataFromSAPDB"/>
+    <hyperlink ref="G49:G51" location="'EVS_SapRSIGetDataFromSAPDB++'!A1" display="EVS_SapRSIGetDataFromSAPDB"/>
+    <hyperlink ref="I52" location="'evs_ProductSearch++'!A1" display="EVS_skuProduct"/>
+    <hyperlink ref="I53" location="'evs_ProductSearch++'!A1" display="EVS_skuProduct"/>
+    <hyperlink ref="G53" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="G54:G56" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="G52" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="H58" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="I58" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="J58" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="K58" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="M58" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="O58" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="P58" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated"/>
+    <hyperlink ref="H57" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="H59" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="J57" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="K57" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="L57" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="N57" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="P57" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="Q57" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="R57" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated"/>
+    <hyperlink ref="O57" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="J59" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="K59" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="L59" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="M59" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="O59" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="Q59" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="R59" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated"/>
+    <hyperlink ref="N59" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="L58" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="M57" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment"/>
+    <hyperlink ref="G57" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="G58" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="G59" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="H60" location="'evs_SubscribeNews_DupEmailID++'!A1" display="evs_SubscribeNews_DupEmailID"/>
+    <hyperlink ref="H61" location="'evs_InvalidEmailNewsLetter++'!A1" display="evs_InvalidEmailNewsLetter"/>
+    <hyperlink ref="H62" location="'evs_SubscribeNewsletter++'!A1" display="ic_SubscribeNewsletter"/>
+    <hyperlink ref="G60:G62" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="H63" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="J63" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="G63" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="H64" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="G64" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="J64" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="K64" location="'evs_RedeemGiftCard++'!A1" display="evs_RedeemGiftCard"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10422,7 +10241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView topLeftCell="A51" workbookViewId="0">
@@ -11469,19 +11288,19 @@
     <cfRule type="duplicateValues" dxfId="241" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"IC_frontend_QA_validUser,IC_frontend_QA_invalidUsername,IC_frontend_QA_invalidPassword,IC_magento_QA,EVS_frontend_QA,EVS_magento_QA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12396,12 +12215,12 @@
     <cfRule type="duplicateValues" dxfId="226" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"IC_frontend_QA_validUser,IC_frontend_QA_invalidUsername,IC_frontend_QA_invalidPassword,IC_magento_QA,EVS_frontend_QA,EVS_magento_QA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12409,7 +12228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -12593,7 +12412,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" location="EVS!A1" display="EVS" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="B3" location="EVS!A1" display="EVS"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12601,7 +12420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA96"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -16497,302 +16316,302 @@
     <cfRule type="duplicateValues" dxfId="186" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
-    <hyperlink ref="H3" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
-    <hyperlink ref="I4" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
-    <hyperlink ref="H4" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0C00-000003000000}"/>
-    <hyperlink ref="I5" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000004000000}"/>
-    <hyperlink ref="H5" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0C00-000005000000}"/>
-    <hyperlink ref="I6" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000006000000}"/>
-    <hyperlink ref="H6" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0C00-000007000000}"/>
-    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000008000000}"/>
-    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000009000000}"/>
-    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0C00-00000A000000}"/>
-    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0C00-00000B000000}"/>
-    <hyperlink ref="J7" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-00000C000000}"/>
-    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00000D000000}"/>
-    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0C00-00000E000000}"/>
-    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0C00-00000F000000}"/>
-    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000010000000}"/>
-    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0C00-000011000000}"/>
-    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000012000000}"/>
-    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0C00-000013000000}"/>
-    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000014000000}"/>
-    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000015000000}"/>
-    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000016000000}"/>
-    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000017000000}"/>
-    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000018000000}"/>
-    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0C00-000019000000}"/>
-    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0C00-00001A000000}"/>
-    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0C00-00001B000000}"/>
-    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0C00-00001C000000}"/>
-    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00001D000000}"/>
-    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00001E000000}"/>
-    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00001F000000}"/>
-    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000020000000}"/>
-    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000021000000}"/>
-    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0C00-000022000000}"/>
-    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000023000000}"/>
-    <hyperlink ref="H27" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-000024000000}"/>
-    <hyperlink ref="I27" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-000025000000}"/>
-    <hyperlink ref="M27" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000026000000}"/>
-    <hyperlink ref="O27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-000027000000}"/>
-    <hyperlink ref="H24" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0C00-000028000000}"/>
-    <hyperlink ref="H25" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0C00-000029000000}"/>
-    <hyperlink ref="H22" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0C00-00002A000000}"/>
-    <hyperlink ref="H23" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0C00-00002B000000}"/>
-    <hyperlink ref="H26" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0C00-00002C000000}"/>
-    <hyperlink ref="J10:J15" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-00002D000000}"/>
-    <hyperlink ref="L17:L21" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-00002E000000}"/>
-    <hyperlink ref="L16" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-00002F000000}"/>
-    <hyperlink ref="J27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-000030000000}"/>
-    <hyperlink ref="K27" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-000031000000}"/>
-    <hyperlink ref="N27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-000032000000}"/>
-    <hyperlink ref="L27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0C00-000033000000}"/>
-    <hyperlink ref="P27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-000034000000}"/>
-    <hyperlink ref="H28" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-000035000000}"/>
-    <hyperlink ref="H30" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-000036000000}"/>
-    <hyperlink ref="I28" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-000037000000}"/>
-    <hyperlink ref="I30" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-000038000000}"/>
-    <hyperlink ref="M28" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000039000000}"/>
-    <hyperlink ref="M30" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00003A000000}"/>
-    <hyperlink ref="O28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-00003B000000}"/>
-    <hyperlink ref="O30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-00003C000000}"/>
-    <hyperlink ref="J28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-00003D000000}"/>
-    <hyperlink ref="J30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-00003E000000}"/>
-    <hyperlink ref="K28" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-00003F000000}"/>
-    <hyperlink ref="K30" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-000040000000}"/>
-    <hyperlink ref="N28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-000041000000}"/>
-    <hyperlink ref="N30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-000042000000}"/>
-    <hyperlink ref="L28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0C00-000043000000}"/>
-    <hyperlink ref="L30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0C00-000044000000}"/>
-    <hyperlink ref="P28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-000045000000}"/>
-    <hyperlink ref="P30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-000046000000}"/>
-    <hyperlink ref="H31" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-000047000000}"/>
-    <hyperlink ref="I31" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-000048000000}"/>
-    <hyperlink ref="L31" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000049000000}"/>
-    <hyperlink ref="O31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-00004A000000}"/>
-    <hyperlink ref="J31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-00004B000000}"/>
-    <hyperlink ref="M31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-00004C000000}"/>
-    <hyperlink ref="K31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0C00-00004D000000}"/>
-    <hyperlink ref="P31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-00004E000000}"/>
-    <hyperlink ref="H29" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-00004F000000}"/>
-    <hyperlink ref="I29" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-000050000000}"/>
-    <hyperlink ref="M29" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000051000000}"/>
-    <hyperlink ref="O29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-000052000000}"/>
-    <hyperlink ref="J29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-000053000000}"/>
-    <hyperlink ref="K29" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-000054000000}"/>
-    <hyperlink ref="N29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-000055000000}"/>
-    <hyperlink ref="L29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0C00-000056000000}"/>
-    <hyperlink ref="P29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-000057000000}"/>
-    <hyperlink ref="H32" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-000058000000}"/>
-    <hyperlink ref="I32" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-000059000000}"/>
-    <hyperlink ref="M32" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00005A000000}"/>
-    <hyperlink ref="J32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-00005B000000}"/>
-    <hyperlink ref="K32" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-00005C000000}"/>
-    <hyperlink ref="N32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-00005D000000}"/>
-    <hyperlink ref="L32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0C00-00005E000000}"/>
-    <hyperlink ref="P32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-00005F000000}"/>
-    <hyperlink ref="Q32" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-000060000000}"/>
-    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000061000000}"/>
-    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000062000000}"/>
-    <hyperlink ref="I37" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-000063000000}"/>
-    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-000064000000}"/>
-    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-000065000000}"/>
-    <hyperlink ref="L33" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000066000000}"/>
-    <hyperlink ref="M33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-000067000000}"/>
-    <hyperlink ref="N33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-000068000000}"/>
-    <hyperlink ref="O33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-000069000000}"/>
-    <hyperlink ref="H33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0C00-00006A000000}"/>
-    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0C00-00006B000000}"/>
-    <hyperlink ref="I34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-00006C000000}"/>
-    <hyperlink ref="J34" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-00006D000000}"/>
-    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00006E000000}"/>
-    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-00006F000000}"/>
-    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-000070000000}"/>
-    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-000071000000}"/>
-    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0C00-000072000000}"/>
-    <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0C00-000073000000}"/>
-    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0C00-000074000000}"/>
-    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0C00-000075000000}"/>
-    <hyperlink ref="I48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0C00-000076000000}"/>
-    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000077000000}"/>
-    <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000078000000}"/>
-    <hyperlink ref="H49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID" xr:uid="{00000000-0004-0000-0C00-000079000000}"/>
-    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-00007A000000}"/>
-    <hyperlink ref="N40" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00007B000000}"/>
-    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-00007C000000}"/>
-    <hyperlink ref="K54" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-00007D000000}"/>
-    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00007E000000}"/>
-    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter" xr:uid="{00000000-0004-0000-0C00-00007F000000}"/>
-    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification" xr:uid="{00000000-0004-0000-0C00-000080000000}"/>
-    <hyperlink ref="O32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-000081000000}"/>
-    <hyperlink ref="K48" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0C00-000082000000}"/>
-    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0C00-000083000000}"/>
-    <hyperlink ref="J48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0C00-000084000000}"/>
-    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0C00-000085000000}"/>
-    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000086000000}"/>
-    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000087000000}"/>
-    <hyperlink ref="H53:H54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0C00-000088000000}"/>
-    <hyperlink ref="I53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0C00-000089000000}"/>
-    <hyperlink ref="J53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0C00-00008A000000}"/>
-    <hyperlink ref="J35" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{00000000-0004-0000-0C00-00008B000000}"/>
-    <hyperlink ref="H36" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-00008C000000}"/>
-    <hyperlink ref="J36" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-00008D000000}"/>
-    <hyperlink ref="K36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-00008E000000}"/>
-    <hyperlink ref="L37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-00008F000000}"/>
-    <hyperlink ref="J37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{00000000-0004-0000-0C00-000090000000}"/>
-    <hyperlink ref="L36" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-000091000000}"/>
-    <hyperlink ref="M37" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-000092000000}"/>
-    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{00000000-0004-0000-0C00-000093000000}"/>
-    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{00000000-0004-0000-0C00-000094000000}"/>
-    <hyperlink ref="H50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy" xr:uid="{00000000-0004-0000-0C00-000095000000}"/>
-    <hyperlink ref="H50:H52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy" xr:uid="{00000000-0004-0000-0C00-000096000000}"/>
-    <hyperlink ref="I2" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-000097000000}"/>
-    <hyperlink ref="L2" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-000098000000}"/>
-    <hyperlink ref="H2" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0C00-000099000000}"/>
-    <hyperlink ref="K2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0C00-00009A000000}"/>
-    <hyperlink ref="L3" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-00009B000000}"/>
-    <hyperlink ref="L5" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-00009C000000}"/>
-    <hyperlink ref="K3" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0C00-00009D000000}"/>
-    <hyperlink ref="K4" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0C00-00009E000000}"/>
-    <hyperlink ref="K5" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0C00-00009F000000}"/>
-    <hyperlink ref="L6" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-0000A0000000}"/>
-    <hyperlink ref="K6" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0C00-0000A1000000}"/>
-    <hyperlink ref="K16" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0C00-0000A2000000}"/>
-    <hyperlink ref="K17:K21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0C00-0000A3000000}"/>
-    <hyperlink ref="J16" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0C00-0000A4000000}"/>
-    <hyperlink ref="J17:J21" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0C00-0000A5000000}"/>
-    <hyperlink ref="J2" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0C00-0000A6000000}"/>
-    <hyperlink ref="J3:J6" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0C00-0000A7000000}"/>
-    <hyperlink ref="K55" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000A8000000}"/>
-    <hyperlink ref="J55" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0C00-0000A9000000}"/>
-    <hyperlink ref="H55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0C00-0000AA000000}"/>
-    <hyperlink ref="L55" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart" xr:uid="{00000000-0004-0000-0C00-0000AB000000}"/>
-    <hyperlink ref="K56" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000AC000000}"/>
-    <hyperlink ref="K57" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000AD000000}"/>
-    <hyperlink ref="G58" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-0000AE000000}"/>
-    <hyperlink ref="J58" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0C00-0000AF000000}"/>
-    <hyperlink ref="H69" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000B0000000}"/>
-    <hyperlink ref="L71" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000B1000000}"/>
-    <hyperlink ref="I71" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0C00-0000B2000000}"/>
-    <hyperlink ref="J71" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0C00-0000B3000000}"/>
-    <hyperlink ref="K71" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0C00-0000B4000000}"/>
-    <hyperlink ref="M71" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail" xr:uid="{00000000-0004-0000-0C00-0000B5000000}"/>
-    <hyperlink ref="N71" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification" xr:uid="{00000000-0004-0000-0C00-0000B6000000}"/>
-    <hyperlink ref="H56:H57" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0C00-0000B7000000}"/>
-    <hyperlink ref="J56:J57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0C00-0000B8000000}"/>
-    <hyperlink ref="H63" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin" xr:uid="{00000000-0004-0000-0C00-0000B9000000}"/>
-    <hyperlink ref="H64" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin" xr:uid="{00000000-0004-0000-0C00-0000BA000000}"/>
-    <hyperlink ref="H70" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000BB000000}"/>
-    <hyperlink ref="H40" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{00000000-0004-0000-0C00-0000BC000000}"/>
-    <hyperlink ref="I40" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000BD000000}"/>
-    <hyperlink ref="I41:I42" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000BE000000}"/>
-    <hyperlink ref="H41:H42" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{00000000-0004-0000-0C00-0000BF000000}"/>
-    <hyperlink ref="K41" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-0000C0000000}"/>
-    <hyperlink ref="K42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-0000C1000000}"/>
-    <hyperlink ref="K40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-0000C2000000}"/>
-    <hyperlink ref="J42" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-0000C3000000}"/>
-    <hyperlink ref="J40:J41" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-0000C4000000}"/>
-    <hyperlink ref="L42" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-0000C5000000}"/>
-    <hyperlink ref="L40:L41" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-0000C6000000}"/>
-    <hyperlink ref="N41" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-0000C7000000}"/>
-    <hyperlink ref="O41" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-0000C8000000}"/>
-    <hyperlink ref="O40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-0000C9000000}"/>
-    <hyperlink ref="O42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-0000CA000000}"/>
-    <hyperlink ref="P42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-0000CB000000}"/>
-    <hyperlink ref="O40:O41" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-0000CC000000}"/>
-    <hyperlink ref="R41" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0C00-0000CD000000}"/>
-    <hyperlink ref="R40" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0C00-0000CE000000}"/>
-    <hyperlink ref="R42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0C00-0000CF000000}"/>
-    <hyperlink ref="R41:R42" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-0000D0000000}"/>
-    <hyperlink ref="M54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0C00-0000D1000000}"/>
-    <hyperlink ref="I55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0C00-0000D2000000}"/>
-    <hyperlink ref="I56:I57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0C00-0000D3000000}"/>
-    <hyperlink ref="L57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0C00-0000D4000000}"/>
-    <hyperlink ref="I54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0C00-0000D5000000}"/>
-    <hyperlink ref="J54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0C00-0000D6000000}"/>
-    <hyperlink ref="L54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0C00-0000D7000000}"/>
-    <hyperlink ref="H74" location="'ic_NavigetoWishlist++'!A1" display="NavigateToWishlist_VerifyLoginPageAppear" xr:uid="{00000000-0004-0000-0C00-0000D8000000}"/>
-    <hyperlink ref="H78" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000D9000000}"/>
-    <hyperlink ref="H79" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000DA000000}"/>
-    <hyperlink ref="G59:G62" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-0000DB000000}"/>
-    <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0C00-0000DC000000}"/>
-    <hyperlink ref="I58" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000DD000000}"/>
-    <hyperlink ref="I59:I62" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000DE000000}"/>
-    <hyperlink ref="H75" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000DF000000}"/>
-    <hyperlink ref="H76:H77" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000E0000000}"/>
-    <hyperlink ref="G80" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-0000E1000000}"/>
-    <hyperlink ref="H80" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0C00-0000E2000000}"/>
-    <hyperlink ref="I80" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000E3000000}"/>
-    <hyperlink ref="L80" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-0000E4000000}"/>
-    <hyperlink ref="G43" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-0000E5000000}"/>
-    <hyperlink ref="H43" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{00000000-0004-0000-0C00-0000E6000000}"/>
-    <hyperlink ref="I43" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000E7000000}"/>
-    <hyperlink ref="G35" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-0000E8000000}"/>
-    <hyperlink ref="I36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{00000000-0004-0000-0C00-0000E9000000}"/>
-    <hyperlink ref="I35" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000EA000000}"/>
-    <hyperlink ref="G85" location="'parrallel_ic_Login++'!A1" display="parrallel_ic_Login" xr:uid="{00000000-0004-0000-0C00-0000EB000000}"/>
-    <hyperlink ref="I88" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-0000EC000000}"/>
-    <hyperlink ref="I89" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-0000ED000000}"/>
-    <hyperlink ref="I90" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-0000EE000000}"/>
-    <hyperlink ref="I91" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-0000EF000000}"/>
-    <hyperlink ref="N92" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-0000F0000000}"/>
-    <hyperlink ref="K92" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-0000F1000000}"/>
-    <hyperlink ref="J92" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-0000F2000000}"/>
-    <hyperlink ref="L92" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-0000F3000000}"/>
-    <hyperlink ref="O92" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-0000F4000000}"/>
-    <hyperlink ref="N93" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-0000F5000000}"/>
-    <hyperlink ref="I93" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000F6000000}"/>
-    <hyperlink ref="K93" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-0000F7000000}"/>
-    <hyperlink ref="J93" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-0000F8000000}"/>
-    <hyperlink ref="L93" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-0000F9000000}"/>
-    <hyperlink ref="O93" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-0000FA000000}"/>
-    <hyperlink ref="G94" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-0000FB000000}"/>
-    <hyperlink ref="H94" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0C00-0000FC000000}"/>
-    <hyperlink ref="I94" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-0000FD000000}"/>
-    <hyperlink ref="K94" location="'validatePaymentOption++'!A1" display="validatePaymentOption" xr:uid="{00000000-0004-0000-0C00-0000FE000000}"/>
-    <hyperlink ref="M93" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0C00-0000FF000000}"/>
-    <hyperlink ref="P92" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-000000010000}"/>
-    <hyperlink ref="G44" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0C00-000001010000}"/>
-    <hyperlink ref="G2:G6" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0C00-000002010000}"/>
-    <hyperlink ref="G22:G33" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0C00-000003010000}"/>
-    <hyperlink ref="G36" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0C00-000004010000}"/>
-    <hyperlink ref="G45:G46" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0C00-000005010000}"/>
-    <hyperlink ref="G49:G57" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0C00-000006010000}"/>
-    <hyperlink ref="G63:G79" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0C00-000007010000}"/>
-    <hyperlink ref="G81:G84" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0C00-000008010000}"/>
-    <hyperlink ref="G86:G93" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0C00-000009010000}"/>
-    <hyperlink ref="G95" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-00000A010000}"/>
-    <hyperlink ref="J95" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-00000B010000}"/>
-    <hyperlink ref="L95" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-00000C010000}"/>
-    <hyperlink ref="M95" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-00000D010000}"/>
-    <hyperlink ref="N95" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0C00-00000E010000}"/>
-    <hyperlink ref="O95" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00000F010000}"/>
-    <hyperlink ref="P95" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-000010010000}"/>
-    <hyperlink ref="S95" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-000011010000}"/>
-    <hyperlink ref="T95" location="'srs_Login++'!A1" display="srs_Login" xr:uid="{00000000-0004-0000-0C00-000012010000}"/>
-    <hyperlink ref="U95" location="'SRSLogonStore++'!A1" display="SRSLogonStore" xr:uid="{00000000-0004-0000-0C00-000013010000}"/>
-    <hyperlink ref="V95" location="'srs_salesOrder_DeliverStatus++'!A1" display="srs_salesOrder_DeliverStatus" xr:uid="{00000000-0004-0000-0C00-000014010000}"/>
-    <hyperlink ref="I95" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0C00-000015010000}"/>
-    <hyperlink ref="R95" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-000016010000}"/>
-    <hyperlink ref="T42" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-000017010000}"/>
-    <hyperlink ref="T40" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-000018010000}"/>
-    <hyperlink ref="T41" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0C00-000019010000}"/>
-    <hyperlink ref="S40" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-00001A010000}"/>
-    <hyperlink ref="N96" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0C00-00001B010000}"/>
-    <hyperlink ref="O96" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0C00-00001C010000}"/>
-    <hyperlink ref="I96" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0C00-00001D010000}"/>
-    <hyperlink ref="K96" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0C00-00001E010000}"/>
-    <hyperlink ref="J96" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0C00-00001F010000}"/>
-    <hyperlink ref="L96" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0C00-000020010000}"/>
-    <hyperlink ref="M96" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0C00-000021010000}"/>
-    <hyperlink ref="G96" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0C00-000022010000}"/>
-    <hyperlink ref="H96" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0C00-000023010000}"/>
-    <hyperlink ref="P96" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0C00-000024010000}"/>
-    <hyperlink ref="Q96" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0C00-000025010000}"/>
-    <hyperlink ref="H88" location="'SapRSIGetDataFromSAPDB++'!A1" display="SapRSIGetDataFromSAPDB" xr:uid="{00000000-0004-0000-0C00-000026010000}"/>
-    <hyperlink ref="H89:H91" location="'SapRSIGetDataFromSAPDB++'!A1" display="SapRSIGetDataFromSAPDB" xr:uid="{00000000-0004-0000-0C00-000027010000}"/>
+    <hyperlink ref="I3" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H3" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="I4" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H4" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="I5" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H5" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="I6" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H6" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
+    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
+    <hyperlink ref="J7" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H27" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I27" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="M27" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="H24" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H25" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H22" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H23" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H26" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="J10:J15" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="L17:L21" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="L16" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="J27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K27" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H28" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H30" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I28" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="I30" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="M28" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M30" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="J28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K28" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="K30" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="L30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="P30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H31" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I31" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L31" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="J31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="M31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H29" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I29" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="M29" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="J29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K29" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H32" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I32" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="M32" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="J32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K32" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="Q32" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="I37" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L33" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="I34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J34" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
+    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="I48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID"/>
+    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="N40" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="K54" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter"/>
+    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification"/>
+    <hyperlink ref="O32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="K48" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="J48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H53:H54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="I53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="J53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="J35" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="H36" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="J36" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="K36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="L37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="L36" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M37" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport"/>
+    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport"/>
+    <hyperlink ref="H50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
+    <hyperlink ref="H50:H52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
+    <hyperlink ref="I2" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="L2" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="H2" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="K2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="L3" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="L5" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="K3" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K4" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K5" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="L6" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="K6" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K16" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K17:K21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="J16" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="J17:J21" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="J2" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="J3:J6" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="K55" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="J55" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="H55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="L55" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart"/>
+    <hyperlink ref="K56" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="K57" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G58" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="J58" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="H69" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="L71" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I71" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="J71" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="K71" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="M71" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail"/>
+    <hyperlink ref="N71" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification"/>
+    <hyperlink ref="H56:H57" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="J56:J57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="H63" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
+    <hyperlink ref="H64" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
+    <hyperlink ref="H70" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H40" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="I40" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I41:I42" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H41:H42" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="K41" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J42" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="J40:J41" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L42" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L40:L41" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N41" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O41" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="O40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="O42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="P42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O40:O41" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="R41" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="R40" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="R42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="R41:R42" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="M54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="I55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I56:I57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="L57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="J54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="L54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="H74" location="'ic_NavigetoWishlist++'!A1" display="NavigateToWishlist_VerifyLoginPageAppear"/>
+    <hyperlink ref="H78" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H79" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G59:G62" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="I58" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I59:I62" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H75" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H76:H77" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G80" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H80" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="I80" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="L80" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G43" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H43" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="I43" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G35" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="I36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="I35" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G85" location="'parrallel_ic_Login++'!A1" display="parrallel_ic_Login"/>
+    <hyperlink ref="I88" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I89" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I90" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I91" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N92" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K92" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J92" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L92" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="O92" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="N93" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I93" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="K93" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J93" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L93" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="O93" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="G94" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H94" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="I94" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="K94" location="'validatePaymentOption++'!A1" display="validatePaymentOption"/>
+    <hyperlink ref="M93" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P92" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="G44" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G2:G6" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G22:G33" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G36" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G45:G46" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G49:G57" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G63:G79" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G81:G84" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G86:G93" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G95" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="J95" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="L95" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="M95" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N95" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O95" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="P95" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="S95" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="T95" location="'srs_Login++'!A1" display="srs_Login"/>
+    <hyperlink ref="U95" location="'SRSLogonStore++'!A1" display="SRSLogonStore"/>
+    <hyperlink ref="V95" location="'srs_salesOrder_DeliverStatus++'!A1" display="srs_salesOrder_DeliverStatus"/>
+    <hyperlink ref="I95" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="R95" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="T42" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="T40" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="T41" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="S40" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="N96" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O96" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="I96" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="K96" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J96" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L96" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M96" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="G96" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H96" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="P96" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="Q96" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H88" location="'SapRSIGetDataFromSAPDB++'!A1" display="SapRSIGetDataFromSAPDB"/>
+    <hyperlink ref="H89:H91" location="'SapRSIGetDataFromSAPDB++'!A1" display="SapRSIGetDataFromSAPDB"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -16800,7 +16619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16836,14 +16655,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16880,14 +16699,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16938,15 +16757,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" location="ZEccSRS-display" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1" location="ZEccSRS-display"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16997,12 +16816,12 @@
     <cfRule type="duplicateValues" dxfId="184" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"IC_frontend_QA_validUser,IC_frontend_QA_invalidUsername,IC_frontend_QA_invalidPassword,IC_magento_QA,EVS_frontend_QA,EVS_magento_QA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -17010,7 +16829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17286,19 +17105,19 @@
     <cfRule type="duplicateValues" dxfId="182" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18" xr:uid="{00000000-0002-0000-1100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18">
       <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17344,14 +17163,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17415,16 +17234,16 @@
     <cfRule type="duplicateValues" dxfId="275" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17498,14 +17317,14 @@
     <cfRule type="duplicateValues" dxfId="180" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17579,16 +17398,16 @@
     <cfRule type="duplicateValues" dxfId="178" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="automation13@gmail.com" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
-    <hyperlink ref="D3" r:id="rId2" display="automation13@gmail.com" xr:uid="{00000000-0004-0000-1400-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId1" display="automation13@gmail.com"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
+    <hyperlink ref="D3" r:id="rId2" display="automation13@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17670,7 +17489,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17794,14 +17613,14 @@
     <cfRule type="duplicateValues" dxfId="171" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17964,19 +17783,19 @@
     <cfRule type="duplicateValues" dxfId="164" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-1700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9">
       <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18171,18 +17990,18 @@
     <cfRule type="duplicateValues" dxfId="159" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2:E3" r:id="rId1" display="watlevi41@gmail.com" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-1800-000001000000}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-1800-000002000000}"/>
-    <hyperlink ref="E4:E7" r:id="rId4" display="MichaelGHand@teleworm.us" xr:uid="{00000000-0004-0000-1800-000003000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1800-000004000000}"/>
+    <hyperlink ref="E2:E3" r:id="rId1" display="watlevi41@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E4:E7" r:id="rId4" display="MichaelGHand@teleworm.us"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18520,16 +18339,16 @@
     <cfRule type="duplicateValues" dxfId="158" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R8" xr:uid="{00000000-0002-0000-1900-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R8">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7 G2:G7 I2:I7 K2:K7 M2:N7 U2:V7" xr:uid="{00000000-0002-0000-1900-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7 G2:G7 I2:I7 K2:K7 M2:N7 U2:V7">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1900-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -18537,7 +18356,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18816,12 +18635,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6 F2:F6 H2:H6 J2:J6 L2:L6 N2:N6" xr:uid="{00000000-0002-0000-1A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6 F2:F6 H2:H6 J2:J6 L2:L6 N2:N6">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18829,7 +18648,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18922,18 +18741,18 @@
     <cfRule type="duplicateValues" dxfId="157" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-1B00-000001000000}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-1B00-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-1B00-000003000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1B00-000004000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19021,15 +18840,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-1C00-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19212,20 +19031,20 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L4" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L4">
       <formula1>"Default(General),Retailer,Wholesale"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K4" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K4">
       <formula1>"Main Website,Everyshop"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H4" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H4">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="F3:F4" r:id="rId2" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F3:F4" r:id="rId2" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -19234,7 +19053,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19309,14 +19128,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19433,14 +19252,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19526,19 +19345,19 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-1F00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
       <formula1>"payUcreditcard"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19651,14 +19470,14 @@
     <cfRule type="duplicateValues" dxfId="156" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19949,11 +19768,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2100-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId2" xr:uid="{00000000-0004-0000-2100-000002000000}"/>
-    <hyperlink ref="O4" r:id="rId3" xr:uid="{00000000-0004-0000-2100-000003000000}"/>
-    <hyperlink ref="O5" r:id="rId4" xr:uid="{00000000-0004-0000-2100-000004000000}"/>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+    <hyperlink ref="O4" r:id="rId3"/>
+    <hyperlink ref="O5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -19961,7 +19780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -20725,28 +20544,28 @@
     <cfRule type="duplicateValues" dxfId="155" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q21:R22 P7 P2:T3 P10:P1048576 T7:T10 Q11:R17 S11:S15" xr:uid="{00000000-0002-0000-2200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q21:R22 P7 P2:T3 P10:P1048576 T7:T10 Q11:R17 S11:S15">
       <formula1>"No,Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3 N11:N1048576" xr:uid="{00000000-0002-0000-2200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3 N11:N1048576">
       <formula1>"ID,Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3 I11:I1048576 M2:M1048576" xr:uid="{00000000-0002-0000-2200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3 I11:I1048576 M2:M1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4:N10" xr:uid="{00000000-0002-0000-2200-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4:N10">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I10 P4:T6 P8:S9 Q7:S7 Q10:S10" xr:uid="{00000000-0002-0000-2200-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I10 P4:T6 P8:S9 Q7:S7 Q10:S10">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L6" xr:uid="{00000000-0002-0000-2200-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L6">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2200-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -20754,14 +20573,14 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22:B22"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -21601,18 +21420,18 @@
     <cfRule type="duplicateValues" dxfId="139" priority="4"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G21 G22" xr:uid="{00000000-0002-0000-2300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G21 G22">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H15 H18:H21 H22" xr:uid="{00000000-0002-0000-2300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H15 H18:H21 H22">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K15 K18:K21 K22" xr:uid="{00000000-0002-0000-2300-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K15 K18:K21 K22">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -21620,21 +21439,21 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2300-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\37601\Documents\JDGroupEVSBranchWorkSpaces\TA421\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA403.xlsx]Products_Category'!#REF!</xm:f>
+            <xm:f>[1]Products_Category!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D23:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2300-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\41066\git\TA635\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA464.xlsx]Products_Category'!#REF!</xm:f>
+            <xm:f>[2]Products_Category!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E10:E15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2300-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\37601\Documents\JDGroupEVSBranchWorkSpaces\TA599_TA600\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA464.xlsx]Products_Category'!#REF!</xm:f>
+            <xm:f>[3]Products_Category!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E18:E21 E22</xm:sqref>
         </x14:dataValidation>
@@ -21645,7 +21464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
@@ -23036,18 +22855,18 @@
     <cfRule type="duplicateValues" dxfId="128" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16" xr:uid="{00000000-0002-0000-2400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G16" xr:uid="{00000000-0002-0000-2400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G16">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K16" xr:uid="{00000000-0002-0000-2400-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K16">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-2400-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -23055,21 +22874,21 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2400-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2400-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>E39:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2400-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\37601\Documents\JDGroupEVSBranchWorkSpaces\TA421\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA403.xlsx]Products_Category'!#REF!</xm:f>
+            <xm:f>[1]Products_Category!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E37:E38</xm:sqref>
         </x14:dataValidation>
@@ -23080,7 +22899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -24337,21 +24156,21 @@
     <cfRule type="duplicateValues" dxfId="122" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32" xr:uid="{00000000-0002-0000-2500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11 Q2:U11 J32 Q32:U32" xr:uid="{00000000-0002-0000-2500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11 Q2:U11 J32 Q32:U32">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O11 O31:O32" xr:uid="{00000000-0002-0000-2500-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O11 O31:O32">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N11 N31:N32" xr:uid="{00000000-0002-0000-2500-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N11 N31:N32">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
+    <hyperlink ref="G7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -24359,7 +24178,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -24447,8 +24266,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-2600-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -24456,7 +24275,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -24782,19 +24601,19 @@
     <cfRule type="duplicateValues" dxfId="274" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18">
       <formula1>"Guest Customer Creation, Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25171,14 +24990,14 @@
     <cfRule type="duplicateValues" dxfId="109" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25397,14 +25216,14 @@
     <cfRule type="duplicateValues" dxfId="107" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2800-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25619,7 +25438,7 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25662,14 +25481,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25718,14 +25537,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-2B00-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25830,7 +25649,7 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25986,7 +25805,7 @@
     <cfRule type="duplicateValues" dxfId="99" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-2D00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
       <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
@@ -25995,7 +25814,7 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26207,22 +26026,22 @@
     <cfRule type="duplicateValues" dxfId="97" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-2E00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
       <formula1>"ExistingUser,logedOn_user"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-2E00-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-2E00-000001000000}"/>
-    <hyperlink ref="E4:E7" r:id="rId3" display="watlevi41@gmail.com" xr:uid="{00000000-0004-0000-2E00-000002000000}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{00000000-0004-0000-2E00-000003000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4:E7" r:id="rId3" display="watlevi41@gmail.com"/>
+    <hyperlink ref="E8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -26614,7 +26433,7 @@
     <cfRule type="duplicateValues" dxfId="91" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-2F00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
     </dataValidation>
   </dataValidations>
@@ -26623,7 +26442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26715,7 +26534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26801,14 +26620,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26871,7 +26690,7 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27027,10 +26846,10 @@
     <cfRule type="duplicateValues" dxfId="86" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{00000000-0002-0000-3200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27039,7 +26858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27155,13 +26974,13 @@
     <cfRule type="duplicateValues" dxfId="84" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-3300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>"ABSA,AFRICAN BANK,BIDVEST.CAPITEC,FNB,INVESTEC,NEDBANK,STANDARD BANK SA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{00000000-0002-0000-3300-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
       <formula1>"English,Afrikaans,Sesotho,Xhosa,Zulu"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27170,7 +26989,7 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27307,7 +27126,7 @@
     <cfRule type="duplicateValues" dxfId="82" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-3400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27315,7 +27134,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-3400-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Preferred Store'!$A$2:$A$71</xm:f>
           </x14:formula1>
@@ -27328,7 +27147,7 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27434,7 +27253,7 @@
     <cfRule type="duplicateValues" dxfId="80" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Domestic Worker,Company Employed,Government Employed,Full-time Housewife,Self Employed - Company Owner,Self Employed - Informal Trader,Student,Unemployed,Pensioner/Retired,Contract Worker,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27444,7 +27263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27690,25 +27509,25 @@
     <cfRule type="duplicateValues" dxfId="78" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3" xr:uid="{00000000-0002-0000-3600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3" xr:uid="{00000000-0002-0000-3600-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3">
       <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3" xr:uid="{00000000-0002-0000-3600-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3">
       <formula1>"African,Asian,Coloured,White,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3" xr:uid="{00000000-0002-0000-3600-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3">
       <formula1>"Single,Married / Civil Partnership,Widowed,Divorced,Separated,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3" xr:uid="{00000000-0002-0000-3600-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3">
       <formula1>"ANC with Accrual,ANC without Accrual,In Community,Customary Union,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3" xr:uid="{00000000-0002-0000-3600-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576" xr:uid="{00000000-0002-0000-3600-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576">
       <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27718,7 +27537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27789,7 +27608,7 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -27844,7 +27663,7 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27935,7 +27754,7 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28585,25 +28404,25 @@
     <cfRule type="duplicateValues" dxfId="68" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10" xr:uid="{00000000-0002-0000-3A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W10 I2:I10 K2:K10 M2:O10 G2:G10 E2:E10 F5:F7" xr:uid="{00000000-0002-0000-3A00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W10 I2:I10 K2:K10 M2:O10 G2:G10 E2:E10 F5:F7">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D6:D7" r:id="rId1" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-3A00-000000000000}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-3A00-000001000000}"/>
-    <hyperlink ref="D2:D4" r:id="rId3" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-3A00-000002000000}"/>
-    <hyperlink ref="D5:D6" r:id="rId4" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-3A00-000003000000}"/>
+    <hyperlink ref="D6:D7" r:id="rId1" display="original2Ic@automationjdg.co.za"/>
+    <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="D2:D4" r:id="rId3" display="original2Ic@automationjdg.co.za"/>
+    <hyperlink ref="D5:D6" r:id="rId4" display="original2Ic@automationjdg.co.za"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -28697,14 +28516,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -29362,7 +29181,7 @@
     <cfRule type="duplicateValues" dxfId="62" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576" xr:uid="{00000000-0002-0000-3B00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -29371,7 +29190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -29825,7 +29644,7 @@
     <cfRule type="duplicateValues" dxfId="60" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3C00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Guest Customer Creation, Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
     </dataValidation>
   </dataValidations>
@@ -29834,7 +29653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -30401,7 +30220,7 @@
     <cfRule type="duplicateValues" dxfId="56" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-3D00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -30409,7 +30228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -30705,19 +30524,19 @@
     <cfRule type="duplicateValues" dxfId="51" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3E00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"payUcreditcard,Cash_Deposits"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-3E00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -31732,18 +31551,18 @@
     <cfRule type="duplicateValues" dxfId="47" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-3F00-000000000000}"/>
-    <hyperlink ref="O3" r:id="rId2" xr:uid="{00000000-0004-0000-3F00-000001000000}"/>
-    <hyperlink ref="O4" r:id="rId3" xr:uid="{00000000-0004-0000-3F00-000002000000}"/>
-    <hyperlink ref="O5" r:id="rId4" xr:uid="{00000000-0004-0000-3F00-000003000000}"/>
-    <hyperlink ref="O8" r:id="rId5" xr:uid="{00000000-0004-0000-3F00-000004000000}"/>
-    <hyperlink ref="O6" r:id="rId6" xr:uid="{00000000-0004-0000-3F00-000005000000}"/>
-    <hyperlink ref="O7" r:id="rId7" xr:uid="{00000000-0004-0000-3F00-000006000000}"/>
-    <hyperlink ref="O9" r:id="rId8" xr:uid="{00000000-0004-0000-3F00-000007000000}"/>
-    <hyperlink ref="O34" r:id="rId9" xr:uid="{00000000-0004-0000-3F00-000008000000}"/>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-3F00-000009000000}"/>
-    <hyperlink ref="O35" r:id="rId10" xr:uid="{00000000-0004-0000-3F00-00000A000000}"/>
-    <hyperlink ref="O36" r:id="rId11" xr:uid="{00000000-0004-0000-3F00-00000B000000}"/>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+    <hyperlink ref="O4" r:id="rId3"/>
+    <hyperlink ref="O5" r:id="rId4"/>
+    <hyperlink ref="O8" r:id="rId5"/>
+    <hyperlink ref="O6" r:id="rId6"/>
+    <hyperlink ref="O7" r:id="rId7"/>
+    <hyperlink ref="O9" r:id="rId8"/>
+    <hyperlink ref="O34" r:id="rId9"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
+    <hyperlink ref="O35" r:id="rId10"/>
+    <hyperlink ref="O36" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
@@ -31751,7 +31570,7 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -31921,7 +31740,7 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -32084,19 +31903,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-4100-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-4100-000001000000}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{00000000-0004-0000-4100-000002000000}"/>
-    <hyperlink ref="H3" r:id="rId4" xr:uid="{00000000-0004-0000-4100-000003000000}"/>
-    <hyperlink ref="J4" r:id="rId5" xr:uid="{00000000-0004-0000-4100-000004000000}"/>
-    <hyperlink ref="H4" r:id="rId6" xr:uid="{00000000-0004-0000-4100-000005000000}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="J3" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId4"/>
+    <hyperlink ref="J4" r:id="rId5"/>
+    <hyperlink ref="H4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -32353,14 +32172,14 @@
     <cfRule type="duplicateValues" dxfId="41" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-4200-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -32697,14 +32516,14 @@
     <cfRule type="duplicateValues" dxfId="37" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4300-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -33017,14 +32836,14 @@
     <cfRule type="duplicateValues" dxfId="33" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4400-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -33140,17 +32959,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="D6" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="C6" r:id="rId6" display="Password@123" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="D3" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="C3" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="D4" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="B6" r:id="rId11" xr:uid="{92846B1C-A7F5-47E9-98C7-A4DFCDB66D91}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D6" r:id="rId2"/>
+    <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId6" display="Password@123"/>
+    <hyperlink ref="D3" r:id="rId7"/>
+    <hyperlink ref="C3" r:id="rId8"/>
+    <hyperlink ref="D4" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
+    <hyperlink ref="B6" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
@@ -33158,7 +32977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -33427,14 +33246,14 @@
     <cfRule type="duplicateValues" dxfId="25" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4500-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -33497,7 +33316,7 @@
 </file>
 
 <file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -33605,12 +33424,10 @@
 </file>
 
 <file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5B2A62-ACC1-49D8-A592-0B4AB924EE0A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -33670,7 +33487,7 @@
     <cfRule type="duplicateValues" dxfId="23" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{669FBBE7-85D2-4882-94D9-F158F768EA28}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
       <formula1>"Reuse,Redeem"</formula1>
     </dataValidation>
   </dataValidations>
@@ -33679,7 +33496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -33779,7 +33596,7 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-4800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>"Reuse,Redeem"</formula1>
     </dataValidation>
   </dataValidations>
@@ -33789,7 +33606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -33873,7 +33690,7 @@
 </file>
 
 <file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34511,44 +34328,44 @@
     <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-4A00-000000000000}"/>
-    <hyperlink ref="F8" r:id="rId2" xr:uid="{00000000-0004-0000-4A00-000001000000}"/>
-    <hyperlink ref="F13" r:id="rId3" display="Password@123" xr:uid="{00000000-0004-0000-4A00-000002000000}"/>
-    <hyperlink ref="F22" r:id="rId4" xr:uid="{00000000-0004-0000-4A00-000003000000}"/>
-    <hyperlink ref="F23" r:id="rId5" xr:uid="{00000000-0004-0000-4A00-000004000000}"/>
-    <hyperlink ref="E13" r:id="rId6" xr:uid="{00000000-0004-0000-4A00-000005000000}"/>
-    <hyperlink ref="F14" r:id="rId7" display="Password@123" xr:uid="{00000000-0004-0000-4A00-000006000000}"/>
-    <hyperlink ref="F12" r:id="rId8" display="Password@123" xr:uid="{00000000-0004-0000-4A00-000007000000}"/>
-    <hyperlink ref="E14" r:id="rId9" xr:uid="{00000000-0004-0000-4A00-000008000000}"/>
-    <hyperlink ref="E17" r:id="rId10" xr:uid="{00000000-0004-0000-4A00-000009000000}"/>
-    <hyperlink ref="F17" r:id="rId11" display="Password@123" xr:uid="{00000000-0004-0000-4A00-00000A000000}"/>
-    <hyperlink ref="E18" r:id="rId12" xr:uid="{00000000-0004-0000-4A00-00000B000000}"/>
-    <hyperlink ref="F18" r:id="rId13" display="Password@123" xr:uid="{00000000-0004-0000-4A00-00000C000000}"/>
-    <hyperlink ref="E20" r:id="rId14" xr:uid="{00000000-0004-0000-4A00-00000D000000}"/>
-    <hyperlink ref="E21" r:id="rId15" xr:uid="{00000000-0004-0000-4A00-00000E000000}"/>
-    <hyperlink ref="E24" r:id="rId16" xr:uid="{00000000-0004-0000-4A00-00000F000000}"/>
-    <hyperlink ref="E25" r:id="rId17" xr:uid="{00000000-0004-0000-4A00-000010000000}"/>
-    <hyperlink ref="E16" r:id="rId18" xr:uid="{00000000-0004-0000-4A00-000011000000}"/>
-    <hyperlink ref="F19" r:id="rId19" display="Password@123" xr:uid="{00000000-0004-0000-4A00-000012000000}"/>
-    <hyperlink ref="E19" r:id="rId20" xr:uid="{00000000-0004-0000-4A00-000013000000}"/>
-    <hyperlink ref="E11" r:id="rId21" xr:uid="{00000000-0004-0000-4A00-000014000000}"/>
-    <hyperlink ref="F11" r:id="rId22" display="Password@123" xr:uid="{00000000-0004-0000-4A00-000015000000}"/>
-    <hyperlink ref="E15" r:id="rId23" xr:uid="{00000000-0004-0000-4A00-000016000000}"/>
-    <hyperlink ref="F15" r:id="rId24" display="Password@123" xr:uid="{00000000-0004-0000-4A00-000017000000}"/>
-    <hyperlink ref="E8" r:id="rId25" xr:uid="{00000000-0004-0000-4A00-000018000000}"/>
-    <hyperlink ref="E10" r:id="rId26" xr:uid="{00000000-0004-0000-4A00-000019000000}"/>
-    <hyperlink ref="F10" r:id="rId27" xr:uid="{00000000-0004-0000-4A00-00001A000000}"/>
-    <hyperlink ref="E9" r:id="rId28" xr:uid="{00000000-0004-0000-4A00-00001B000000}"/>
-    <hyperlink ref="F9" r:id="rId29" xr:uid="{00000000-0004-0000-4A00-00001C000000}"/>
-    <hyperlink ref="F3:F7" r:id="rId30" display="Password@123" xr:uid="{00000000-0004-0000-4A00-00001D000000}"/>
-    <hyperlink ref="F3" r:id="rId31" xr:uid="{00000000-0004-0000-4A00-00001E000000}"/>
-    <hyperlink ref="F4" r:id="rId32" xr:uid="{00000000-0004-0000-4A00-00001F000000}"/>
-    <hyperlink ref="F5" r:id="rId33" xr:uid="{00000000-0004-0000-4A00-000020000000}"/>
-    <hyperlink ref="F6" r:id="rId34" xr:uid="{00000000-0004-0000-4A00-000021000000}"/>
-    <hyperlink ref="F7" r:id="rId35" xr:uid="{00000000-0004-0000-4A00-000022000000}"/>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4A00-000023000000}"/>
-    <hyperlink ref="F29" r:id="rId36" display="Password@123" xr:uid="{00000000-0004-0000-4A00-000024000000}"/>
-    <hyperlink ref="E29" r:id="rId37" xr:uid="{00000000-0004-0000-4A00-000025000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="F13" r:id="rId3" display="Password@123"/>
+    <hyperlink ref="F22" r:id="rId4"/>
+    <hyperlink ref="F23" r:id="rId5"/>
+    <hyperlink ref="E13" r:id="rId6"/>
+    <hyperlink ref="F14" r:id="rId7" display="Password@123"/>
+    <hyperlink ref="F12" r:id="rId8" display="Password@123"/>
+    <hyperlink ref="E14" r:id="rId9"/>
+    <hyperlink ref="E17" r:id="rId10"/>
+    <hyperlink ref="F17" r:id="rId11" display="Password@123"/>
+    <hyperlink ref="E18" r:id="rId12"/>
+    <hyperlink ref="F18" r:id="rId13" display="Password@123"/>
+    <hyperlink ref="E20" r:id="rId14"/>
+    <hyperlink ref="E21" r:id="rId15"/>
+    <hyperlink ref="E24" r:id="rId16"/>
+    <hyperlink ref="E25" r:id="rId17"/>
+    <hyperlink ref="E16" r:id="rId18"/>
+    <hyperlink ref="F19" r:id="rId19" display="Password@123"/>
+    <hyperlink ref="E19" r:id="rId20"/>
+    <hyperlink ref="E11" r:id="rId21"/>
+    <hyperlink ref="F11" r:id="rId22" display="Password@123"/>
+    <hyperlink ref="E15" r:id="rId23"/>
+    <hyperlink ref="F15" r:id="rId24" display="Password@123"/>
+    <hyperlink ref="E8" r:id="rId25"/>
+    <hyperlink ref="E10" r:id="rId26"/>
+    <hyperlink ref="F10" r:id="rId27"/>
+    <hyperlink ref="E9" r:id="rId28"/>
+    <hyperlink ref="F9" r:id="rId29"/>
+    <hyperlink ref="F3:F7" r:id="rId30" display="Password@123"/>
+    <hyperlink ref="F3" r:id="rId31"/>
+    <hyperlink ref="F4" r:id="rId32"/>
+    <hyperlink ref="F5" r:id="rId33"/>
+    <hyperlink ref="F6" r:id="rId34"/>
+    <hyperlink ref="F7" r:id="rId35"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
+    <hyperlink ref="F29" r:id="rId36" display="Password@123"/>
+    <hyperlink ref="E29" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId38"/>
@@ -34556,7 +34373,7 @@
 </file>
 
 <file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34800,14 +34617,14 @@
     <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4B00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -34894,15 +34711,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-4C00-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-4C00-000001000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34958,7 +34775,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -35392,14 +35209,14 @@
     <cfRule type="duplicateValues" dxfId="272" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -35500,14 +35317,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-4E00-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -35631,8 +35448,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Welc0me@2021" xr:uid="{00000000-0004-0000-4F00-000000000000}"/>
-    <hyperlink ref="F6" r:id="rId2" xr:uid="{00000000-0004-0000-4F00-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="Welc0me@2021"/>
+    <hyperlink ref="F6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -35640,7 +35457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -35767,9 +35584,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-5000-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-5000-000001000000}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-5000-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -35777,7 +35594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -35834,7 +35651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36303,17 +36120,17 @@
     <cfRule type="duplicateValues" dxfId="0" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-5200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G4 F5:F1048576" xr:uid="{00000000-0002-0000-5200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G4 F5:F1048576">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-5200-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-5200-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-5200-000002000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -36322,7 +36139,7 @@
 </file>
 
 <file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36363,7 +36180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36467,7 +36284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36671,7 +36488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36775,7 +36592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36879,7 +36696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37520,7 +37337,7 @@
     <cfRule type="duplicateValues" dxfId="262" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -37528,7 +37345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37901,7 +37718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -38005,7 +37822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">
@@ -38109,21 +37926,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -38276,14 +38093,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -38296,6 +38105,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>